<commit_message>
corrected call stack logging added few more configs
</commit_message>
<xml_diff>
--- a/config/test-words.xlsx
+++ b/config/test-words.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
   <si>
     <t>#VALUE LOG</t>
   </si>
@@ -95,19 +95,25 @@
     <t>debug</t>
   </si>
   <si>
-    <t>H3U</t>
-  </si>
-  <si>
-    <t>H4U</t>
-  </si>
-  <si>
-    <t>H5U</t>
-  </si>
-  <si>
     <t>H2F</t>
   </si>
   <si>
     <t>H4F</t>
+  </si>
+  <si>
+    <t>H6F</t>
+  </si>
+  <si>
+    <t>H8U</t>
+  </si>
+  <si>
+    <t>H9U</t>
+  </si>
+  <si>
+    <t>H10U</t>
+  </si>
+  <si>
+    <t>ctr</t>
   </si>
 </sst>
 </file>
@@ -934,10 +940,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I30"/>
+  <dimension ref="A1:J30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14:I16"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -947,12 +953,12 @@
     <col min="9" max="9" width="12.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -963,7 +969,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>7</v>
       </c>
@@ -974,7 +980,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -982,22 +988,22 @@
         <v>502</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C5">
         <v>70</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C6">
         <v>50</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C7">
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>20</v>
       </c>
@@ -1005,7 +1011,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>4</v>
       </c>
@@ -1013,7 +1019,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>22</v>
       </c>
@@ -1021,14 +1027,14 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="12" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="12" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>8</v>
       </c>
@@ -1056,8 +1062,11 @@
       <c r="I14" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J14" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>15</v>
       </c>
@@ -1068,22 +1077,25 @@
         <v>17</v>
       </c>
       <c r="E15" t="s">
+        <v>23</v>
+      </c>
+      <c r="F15" t="s">
+        <v>24</v>
+      </c>
+      <c r="G15" t="s">
+        <v>25</v>
+      </c>
+      <c r="H15" t="s">
         <v>26</v>
       </c>
-      <c r="F15" t="s">
+      <c r="I15" t="s">
         <v>27</v>
       </c>
-      <c r="G15" t="s">
-        <v>23</v>
-      </c>
-      <c r="H15" t="s">
-        <v>24</v>
-      </c>
-      <c r="I15" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J15" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>10000</v>
       </c>
@@ -1111,6 +1123,10 @@
       </c>
       <c r="I16">
         <v>5</v>
+      </c>
+      <c r="J16">
+        <f>C16</f>
+        <v>1</v>
       </c>
     </row>
     <row r="17" spans="6:7" x14ac:dyDescent="0.25">

</xml_diff>